<commit_message>
add equip quality config
</commit_message>
<xml_diff>
--- a/Excel/SkillRuneConfig.xlsx
+++ b/Excel/SkillRuneConfig.xlsx
@@ -142,7 +142,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="40">
   <si>
     <t>_ID</t>
   </si>
@@ -153,7 +153,7 @@
     <t>词条名字</t>
   </si>
   <si>
-    <t>#说明</t>
+    <t>套装ID</t>
   </si>
   <si>
     <t>技能描述</t>
@@ -193,6 +193,9 @@
   </si>
   <si>
     <t>Name</t>
+  </si>
+  <si>
+    <t>SuitId</t>
   </si>
   <si>
     <t>Des</t>
@@ -1228,12 +1231,12 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="C3:P10"/>
+  <dimension ref="C3:P15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="5" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="E16" sqref="E16"/>
+      <selection pane="bottomLeft" activeCell="E23" sqref="E23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25"/>
@@ -1305,78 +1308,82 @@
       <c r="E4" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="F4" s="3"/>
+      <c r="F4" s="3" t="s">
+        <v>17</v>
+      </c>
       <c r="G4" s="3" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="H4" s="3" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="I4" s="3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="J4" s="3" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="K4" s="3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="L4" s="3" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="M4" s="3" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="N4" s="3" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="O4" s="3" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="P4" s="3" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
     </row>
     <row r="5" spans="3:16">
       <c r="C5" s="3" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="E5" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="F5" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="F5" s="3"/>
       <c r="G5" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="H5" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="H5" s="3" t="s">
-        <v>27</v>
-      </c>
       <c r="I5" s="3" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="J5" s="3" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="K5" s="3" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="L5" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="M5" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="M5" s="3" t="s">
-        <v>27</v>
-      </c>
       <c r="N5" s="3" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="O5" s="3" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="P5" s="3" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
     </row>
     <row r="6" s="1" customFormat="1" spans="3:16">
@@ -1387,10 +1394,13 @@
         <v>2001</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>29</v>
+        <v>30</v>
+      </c>
+      <c r="F6" s="1">
+        <v>20011</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="H6" s="1">
         <v>99</v>
@@ -1404,7 +1414,6 @@
       <c r="K6" s="1">
         <v>0</v>
       </c>
-      <c r="L6" s="1"/>
       <c r="M6" s="1">
         <v>0</v>
       </c>
@@ -1426,10 +1435,13 @@
         <v>2001</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>31</v>
+        <v>32</v>
+      </c>
+      <c r="F7" s="1">
+        <v>20011</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="H7" s="1">
         <v>3</v>
@@ -1464,10 +1476,13 @@
         <v>2001</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>33</v>
+        <v>34</v>
+      </c>
+      <c r="F8" s="1">
+        <v>20011</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="H8" s="1">
         <v>1</v>
@@ -1502,10 +1517,13 @@
         <v>2001</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>35</v>
+        <v>36</v>
+      </c>
+      <c r="F9" s="1">
+        <v>20011</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="H9" s="1">
         <v>3</v>
@@ -1540,10 +1558,13 @@
         <v>2001</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>37</v>
+        <v>38</v>
+      </c>
+      <c r="F10" s="1">
+        <v>20011</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="H10" s="1">
         <v>99</v>
@@ -1567,6 +1588,211 @@
         <v>100</v>
       </c>
       <c r="P10" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" s="1" customFormat="1" spans="3:16">
+      <c r="C11" s="1">
+        <v>20021</v>
+      </c>
+      <c r="D11" s="1">
+        <v>2001</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="F11" s="1">
+        <v>20012</v>
+      </c>
+      <c r="G11" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="H11" s="1">
+        <v>99</v>
+      </c>
+      <c r="I11" s="1">
+        <v>0</v>
+      </c>
+      <c r="J11" s="1">
+        <v>0</v>
+      </c>
+      <c r="K11" s="1">
+        <v>0</v>
+      </c>
+      <c r="M11" s="1">
+        <v>0</v>
+      </c>
+      <c r="N11" s="1">
+        <v>20</v>
+      </c>
+      <c r="O11" s="1">
+        <v>0</v>
+      </c>
+      <c r="P11" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" s="1" customFormat="1" spans="3:16">
+      <c r="C12" s="1">
+        <v>20022</v>
+      </c>
+      <c r="D12" s="1">
+        <v>2001</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="F12" s="1">
+        <v>20012</v>
+      </c>
+      <c r="G12" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="H12" s="1">
+        <v>3</v>
+      </c>
+      <c r="I12" s="1">
+        <v>0</v>
+      </c>
+      <c r="J12" s="1">
+        <v>0</v>
+      </c>
+      <c r="K12" s="1">
+        <v>0</v>
+      </c>
+      <c r="M12" s="1">
+        <v>1</v>
+      </c>
+      <c r="N12" s="1">
+        <v>0</v>
+      </c>
+      <c r="O12" s="1">
+        <v>0</v>
+      </c>
+      <c r="P12" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" s="1" customFormat="1" spans="3:16">
+      <c r="C13" s="1">
+        <v>20023</v>
+      </c>
+      <c r="D13" s="1">
+        <v>2001</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="F13" s="1">
+        <v>20012</v>
+      </c>
+      <c r="G13" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="H13" s="1">
+        <v>1</v>
+      </c>
+      <c r="I13" s="1">
+        <v>1</v>
+      </c>
+      <c r="J13" s="1">
+        <v>0</v>
+      </c>
+      <c r="K13" s="1">
+        <v>0</v>
+      </c>
+      <c r="M13" s="1">
+        <v>0</v>
+      </c>
+      <c r="N13" s="1">
+        <v>0</v>
+      </c>
+      <c r="O13" s="1">
+        <v>0</v>
+      </c>
+      <c r="P13" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" s="1" customFormat="1" spans="3:16">
+      <c r="C14" s="1">
+        <v>20024</v>
+      </c>
+      <c r="D14" s="1">
+        <v>2001</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="F14" s="1">
+        <v>20012</v>
+      </c>
+      <c r="G14" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="H14" s="1">
+        <v>3</v>
+      </c>
+      <c r="I14" s="1">
+        <v>0</v>
+      </c>
+      <c r="J14" s="1">
+        <v>0</v>
+      </c>
+      <c r="K14" s="1">
+        <v>0</v>
+      </c>
+      <c r="M14" s="1">
+        <v>0</v>
+      </c>
+      <c r="N14" s="1">
+        <v>0</v>
+      </c>
+      <c r="O14" s="1">
+        <v>0</v>
+      </c>
+      <c r="P14" s="1">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="15" s="1" customFormat="1" spans="3:16">
+      <c r="C15" s="1">
+        <v>20025</v>
+      </c>
+      <c r="D15" s="1">
+        <v>2001</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="F15" s="1">
+        <v>20012</v>
+      </c>
+      <c r="G15" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="H15" s="1">
+        <v>99</v>
+      </c>
+      <c r="I15" s="1">
+        <v>0</v>
+      </c>
+      <c r="J15" s="1">
+        <v>0</v>
+      </c>
+      <c r="K15" s="1">
+        <v>0</v>
+      </c>
+      <c r="M15" s="1">
+        <v>0</v>
+      </c>
+      <c r="N15" s="1">
+        <v>0</v>
+      </c>
+      <c r="O15" s="1">
+        <v>100</v>
+      </c>
+      <c r="P15" s="1">
         <v>0</v>
       </c>
     </row>

</xml_diff>